<commit_message>
save work (not working)
</commit_message>
<xml_diff>
--- a/documentation/dev/files/wind generation.xlsx
+++ b/documentation/dev/files/wind generation.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -147,192 +146,192 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.800541092008299</c:v>
+                  <c:v>15.360292987400241</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.261317266311757</c:v>
+                  <c:v>15.997748830366756</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.850682442323233</c:v>
+                  <c:v>16.458864275017021</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16.131041204054306</c:v>
+                  <c:v>16.846578143651026</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.121855684024684</c:v>
+                  <c:v>16.224129167562197</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.301537552249211</c:v>
+                  <c:v>17.081919742998902</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.718729185173725</c:v>
+                  <c:v>16.444110547563383</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14.505878406835357</c:v>
+                  <c:v>16.59196139442836</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.206680587792787</c:v>
+                  <c:v>15.731419847922977</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>15.011344507310829</c:v>
+                  <c:v>14.927859019320399</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14.331190582856889</c:v>
+                  <c:v>15.532424157724424</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14.124496886506426</c:v>
+                  <c:v>16.196987421720394</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14.473000803349887</c:v>
+                  <c:v>16.539739541082909</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15.392577433117602</c:v>
+                  <c:v>15.422576761713531</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.45060492242577</c:v>
+                  <c:v>16.352394707924901</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15.586012613777458</c:v>
+                  <c:v>15.398068802271791</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.701170170045142</c:v>
+                  <c:v>16.631647438745137</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14.418710848969761</c:v>
+                  <c:v>15.151123211714976</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14.201614836207733</c:v>
+                  <c:v>16.511168075096734</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>14.12387747436677</c:v>
+                  <c:v>16.630107035414323</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13.548775597603345</c:v>
+                  <c:v>17.008083009475531</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>13.552419677988862</c:v>
+                  <c:v>16.011959758549803</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>14.285423493271471</c:v>
+                  <c:v>17.503561284776044</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>14.029328692207741</c:v>
+                  <c:v>17.884412364648522</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>14.477316228401135</c:v>
+                  <c:v>18.213178942235761</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>15.386657962499671</c:v>
+                  <c:v>17.563149184145274</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>15.94803114810601</c:v>
+                  <c:v>18.348705158254099</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>15.93064120741292</c:v>
+                  <c:v>16.825630714906172</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15.091026029861903</c:v>
+                  <c:v>15.331165243797123</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>14.717176318940787</c:v>
+                  <c:v>16.488709361856117</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>16.199258293635506</c:v>
+                  <c:v>16.208129944785931</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>16.778471625286883</c:v>
+                  <c:v>18.149762488736261</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>18.921616155872087</c:v>
+                  <c:v>16.886771416427646</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>18.140255440025431</c:v>
+                  <c:v>17.584231401942805</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>19.082730864376831</c:v>
+                  <c:v>17.738174270511198</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>19.283436950412959</c:v>
+                  <c:v>17.590633631868553</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>20.532178196998441</c:v>
+                  <c:v>17.314708771974292</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>20.558784822901146</c:v>
+                  <c:v>18.088356398608962</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>20.711624327118695</c:v>
+                  <c:v>19.271079064255847</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>19.601504438970728</c:v>
+                  <c:v>19.249163300366952</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>19.600748146126435</c:v>
+                  <c:v>19.835410928668029</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>19.831853561742133</c:v>
+                  <c:v>19.463558995430859</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>18.621499155428772</c:v>
+                  <c:v>19.803468243509077</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>20.185660176957295</c:v>
+                  <c:v>20.549456090462115</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>20.013749324739774</c:v>
+                  <c:v>20.816126104682439</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>19.987077516497362</c:v>
+                  <c:v>21.718547610700885</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>19.646068420129687</c:v>
+                  <c:v>21.82694216613152</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>20.700741011162304</c:v>
+                  <c:v>20.723825551845287</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>21.920833389720336</c:v>
+                  <c:v>20.158187124646801</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>21.981141041583673</c:v>
+                  <c:v>20.613869947741943</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>20.664492616574361</c:v>
+                  <c:v>20.723031107517805</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>19.129898968726998</c:v>
+                  <c:v>20.68520748055197</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>18.690116028792804</c:v>
+                  <c:v>22.068904024297414</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>16.677338981522688</c:v>
+                  <c:v>24.011548346851328</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>17.138390850766015</c:v>
+                  <c:v>21.966565210104037</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>17.557842812418617</c:v>
+                  <c:v>21.396425223195621</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>17.457280314545315</c:v>
+                  <c:v>20.00838906661874</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>17.58396063135708</c:v>
+                  <c:v>20.586970064562344</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>18.85673089605644</c:v>
+                  <c:v>21.096799394188476</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="107608320"/>
-        <c:axId val="119472128"/>
+        <c:axId val="113126400"/>
+        <c:axId val="118723328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="107608320"/>
+        <c:axId val="113126400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -348,13 +347,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="119472128"/>
+        <c:crossAx val="118723328"/>
         <c:crosses val="autoZero"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="119472128"/>
+        <c:axId val="118723328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80"/>
@@ -387,7 +386,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="107608320"/>
+        <c:crossAx val="113126400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -396,7 +395,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -419,7 +418,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -7581,73 +7580,73 @@
     <row r="254" spans="1:8" ht="15.75" customHeight="1">
       <c r="G254">
         <f t="shared" ref="G254:G265" ca="1" si="1">G253*EXP($I$13+$I$10*NORMSINV(RAND()))</f>
-        <v>219.06531118507581</v>
+        <v>220.20291389160218</v>
       </c>
     </row>
     <row r="255" spans="1:8" ht="15.75" customHeight="1">
       <c r="G255">
         <f t="shared" ca="1" si="1"/>
-        <v>220.98331590244936</v>
+        <v>233.97344037698909</v>
       </c>
     </row>
     <row r="256" spans="1:8" ht="15.75" customHeight="1">
       <c r="G256">
         <f t="shared" ca="1" si="1"/>
-        <v>216.68788151339101</v>
+        <v>234.8117744407227</v>
       </c>
     </row>
     <row r="257" spans="7:7" ht="15.75" customHeight="1">
       <c r="G257">
         <f t="shared" ca="1" si="1"/>
-        <v>226.30581961529725</v>
+        <v>238.06146637100349</v>
       </c>
     </row>
     <row r="258" spans="7:7" ht="15.75" customHeight="1">
       <c r="G258">
         <f t="shared" ca="1" si="1"/>
-        <v>224.82061044311837</v>
+        <v>249.6404829573529</v>
       </c>
     </row>
     <row r="259" spans="7:7" ht="15.75" customHeight="1">
       <c r="G259">
         <f t="shared" ca="1" si="1"/>
-        <v>220.11916185942192</v>
+        <v>249.83394141537124</v>
       </c>
     </row>
     <row r="260" spans="7:7" ht="15.75" customHeight="1">
       <c r="G260">
         <f t="shared" ca="1" si="1"/>
-        <v>214.05003280818534</v>
+        <v>243.30089834725263</v>
       </c>
     </row>
     <row r="261" spans="7:7" ht="15.75" customHeight="1">
       <c r="G261">
         <f t="shared" ca="1" si="1"/>
-        <v>211.38438417998472</v>
+        <v>240.84383360852456</v>
       </c>
     </row>
     <row r="262" spans="7:7" ht="15.75" customHeight="1">
       <c r="G262">
         <f t="shared" ca="1" si="1"/>
-        <v>213.12209999393093</v>
+        <v>241.50950885614077</v>
       </c>
     </row>
     <row r="263" spans="7:7" ht="15.75" customHeight="1">
       <c r="G263">
         <f t="shared" ca="1" si="1"/>
-        <v>219.01033869227689</v>
+        <v>239.51497053073027</v>
       </c>
     </row>
     <row r="264" spans="7:7" ht="15.75" customHeight="1">
       <c r="G264">
         <f t="shared" ca="1" si="1"/>
-        <v>227.47654668816261</v>
+        <v>234.29189424751291</v>
       </c>
     </row>
     <row r="265" spans="7:7" ht="15.75" customHeight="1">
       <c r="G265">
         <f t="shared" ca="1" si="1"/>
-        <v>226.78239441772257</v>
+        <v>243.10396998321741</v>
       </c>
     </row>
   </sheetData>
@@ -7659,8 +7658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -7699,7 +7698,7 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B60" ca="1" si="0">B1*EXP($G$4+$G$3*NORMSINV(RAND()))</f>
-        <v>14.800541092008299</v>
+        <v>15.360292987400241</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -7720,7 +7719,7 @@
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>15.261317266311757</v>
+        <v>15.997748830366756</v>
       </c>
       <c r="E3">
         <v>2.4401961635863837E-2</v>
@@ -7739,7 +7738,7 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>16.850682442323233</v>
+        <v>16.458864275017021</v>
       </c>
       <c r="E4">
         <v>-2.3615325941041872E-4</v>
@@ -7749,11 +7748,11 @@
       </c>
       <c r="G4" s="1">
         <f ca="1">0.0005*(0.5-RAND())*(3375/G5^3)</f>
-        <v>-1.8919611828583304E-4</v>
+        <v>-1.0794875962786832E-4</v>
       </c>
       <c r="H4" s="1">
         <f ca="1">0.5-(RAND())</f>
-        <v>-0.12720187430130503</v>
+        <v>-0.33604563748369554</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1">
@@ -7762,7 +7761,7 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>16.131041204054306</v>
+        <v>16.846578143651026</v>
       </c>
       <c r="E5" s="3">
         <v>7</v>
@@ -7780,7 +7779,7 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>16.121855684024684</v>
+        <v>16.224129167562197</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>16</v>
@@ -7792,7 +7791,7 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>16.301537552249211</v>
+        <v>17.081919742998902</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1">
@@ -7801,7 +7800,7 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>15.718729185173725</v>
+        <v>16.444110547563383</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1">
@@ -7810,7 +7809,7 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>14.505878406835357</v>
+        <v>16.59196139442836</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1">
@@ -7819,7 +7818,7 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>14.206680587792787</v>
+        <v>15.731419847922977</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1">
@@ -7828,7 +7827,7 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>15.011344507310829</v>
+        <v>14.927859019320399</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1">
@@ -7837,7 +7836,7 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>14.331190582856889</v>
+        <v>15.532424157724424</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1">
@@ -7846,7 +7845,7 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>14.124496886506426</v>
+        <v>16.196987421720394</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1">
@@ -7855,7 +7854,7 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>14.473000803349887</v>
+        <v>16.539739541082909</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1">
@@ -7864,7 +7863,7 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>15.392577433117602</v>
+        <v>15.422576761713531</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1">
@@ -7873,7 +7872,7 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>15.45060492242577</v>
+        <v>16.352394707924901</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1">
@@ -7882,7 +7881,7 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>15.586012613777458</v>
+        <v>15.398068802271791</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1">
@@ -7891,7 +7890,7 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>14.701170170045142</v>
+        <v>16.631647438745137</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" customHeight="1">
@@ -7900,7 +7899,7 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>14.418710848969761</v>
+        <v>15.151123211714976</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" customHeight="1">
@@ -7909,7 +7908,7 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>14.201614836207733</v>
+        <v>16.511168075096734</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" customHeight="1">
@@ -7918,241 +7917,241 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>14.12387747436677</v>
+        <v>16.630107035414323</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1">
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>13.548775597603345</v>
+        <v>17.008083009475531</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" customHeight="1">
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>13.552419677988862</v>
+        <v>16.011959758549803</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" customHeight="1">
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>14.285423493271471</v>
+        <v>17.503561284776044</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" customHeight="1">
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>14.029328692207741</v>
+        <v>17.884412364648522</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" customHeight="1">
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>14.477316228401135</v>
+        <v>18.213178942235761</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" customHeight="1">
       <c r="B27">
         <f t="shared" ca="1" si="0"/>
-        <v>15.386657962499671</v>
+        <v>17.563149184145274</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" customHeight="1">
       <c r="B28">
         <f t="shared" ca="1" si="0"/>
-        <v>15.94803114810601</v>
+        <v>18.348705158254099</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" customHeight="1">
       <c r="B29">
         <f t="shared" ca="1" si="0"/>
-        <v>15.93064120741292</v>
+        <v>16.825630714906172</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" customHeight="1">
       <c r="B30">
         <f t="shared" ca="1" si="0"/>
-        <v>15.091026029861903</v>
+        <v>15.331165243797123</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" customHeight="1">
       <c r="B31">
         <f t="shared" ca="1" si="0"/>
-        <v>14.717176318940787</v>
+        <v>16.488709361856117</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" customHeight="1">
       <c r="B32">
         <f t="shared" ca="1" si="0"/>
-        <v>16.199258293635506</v>
+        <v>16.208129944785931</v>
       </c>
     </row>
     <row r="33" spans="2:2" ht="15.75" customHeight="1">
       <c r="B33">
         <f t="shared" ca="1" si="0"/>
-        <v>16.778471625286883</v>
+        <v>18.149762488736261</v>
       </c>
     </row>
     <row r="34" spans="2:2" ht="15.75" customHeight="1">
       <c r="B34">
         <f t="shared" ca="1" si="0"/>
-        <v>18.921616155872087</v>
+        <v>16.886771416427646</v>
       </c>
     </row>
     <row r="35" spans="2:2" ht="15.75" customHeight="1">
       <c r="B35">
         <f t="shared" ca="1" si="0"/>
-        <v>18.140255440025431</v>
+        <v>17.584231401942805</v>
       </c>
     </row>
     <row r="36" spans="2:2" ht="15.75" customHeight="1">
       <c r="B36">
         <f t="shared" ca="1" si="0"/>
-        <v>19.082730864376831</v>
+        <v>17.738174270511198</v>
       </c>
     </row>
     <row r="37" spans="2:2" ht="15.75" customHeight="1">
       <c r="B37">
         <f t="shared" ca="1" si="0"/>
-        <v>19.283436950412959</v>
+        <v>17.590633631868553</v>
       </c>
     </row>
     <row r="38" spans="2:2" ht="15.75" customHeight="1">
       <c r="B38">
         <f t="shared" ca="1" si="0"/>
-        <v>20.532178196998441</v>
+        <v>17.314708771974292</v>
       </c>
     </row>
     <row r="39" spans="2:2" ht="15.75" customHeight="1">
       <c r="B39">
         <f t="shared" ca="1" si="0"/>
-        <v>20.558784822901146</v>
+        <v>18.088356398608962</v>
       </c>
     </row>
     <row r="40" spans="2:2" ht="15.75" customHeight="1">
       <c r="B40">
         <f t="shared" ca="1" si="0"/>
-        <v>20.711624327118695</v>
+        <v>19.271079064255847</v>
       </c>
     </row>
     <row r="41" spans="2:2" ht="15.75" customHeight="1">
       <c r="B41">
         <f t="shared" ca="1" si="0"/>
-        <v>19.601504438970728</v>
+        <v>19.249163300366952</v>
       </c>
     </row>
     <row r="42" spans="2:2" ht="15.75" customHeight="1">
       <c r="B42">
         <f t="shared" ca="1" si="0"/>
-        <v>19.600748146126435</v>
+        <v>19.835410928668029</v>
       </c>
     </row>
     <row r="43" spans="2:2" ht="15.75" customHeight="1">
       <c r="B43">
         <f t="shared" ca="1" si="0"/>
-        <v>19.831853561742133</v>
+        <v>19.463558995430859</v>
       </c>
     </row>
     <row r="44" spans="2:2" ht="15.75" customHeight="1">
       <c r="B44">
         <f t="shared" ca="1" si="0"/>
-        <v>18.621499155428772</v>
+        <v>19.803468243509077</v>
       </c>
     </row>
     <row r="45" spans="2:2" ht="15.75" customHeight="1">
       <c r="B45">
         <f t="shared" ca="1" si="0"/>
-        <v>20.185660176957295</v>
+        <v>20.549456090462115</v>
       </c>
     </row>
     <row r="46" spans="2:2" ht="15.75" customHeight="1">
       <c r="B46">
         <f t="shared" ca="1" si="0"/>
-        <v>20.013749324739774</v>
+        <v>20.816126104682439</v>
       </c>
     </row>
     <row r="47" spans="2:2" ht="15.75" customHeight="1">
       <c r="B47">
         <f t="shared" ca="1" si="0"/>
-        <v>19.987077516497362</v>
+        <v>21.718547610700885</v>
       </c>
     </row>
     <row r="48" spans="2:2" ht="15.75" customHeight="1">
       <c r="B48">
         <f t="shared" ca="1" si="0"/>
-        <v>19.646068420129687</v>
+        <v>21.82694216613152</v>
       </c>
     </row>
     <row r="49" spans="2:2" ht="15.75" customHeight="1">
       <c r="B49">
         <f t="shared" ca="1" si="0"/>
-        <v>20.700741011162304</v>
+        <v>20.723825551845287</v>
       </c>
     </row>
     <row r="50" spans="2:2" ht="15.75" customHeight="1">
       <c r="B50">
         <f t="shared" ca="1" si="0"/>
-        <v>21.920833389720336</v>
+        <v>20.158187124646801</v>
       </c>
     </row>
     <row r="51" spans="2:2" ht="15.75" customHeight="1">
       <c r="B51">
         <f t="shared" ca="1" si="0"/>
-        <v>21.981141041583673</v>
+        <v>20.613869947741943</v>
       </c>
     </row>
     <row r="52" spans="2:2" ht="15.75" customHeight="1">
       <c r="B52">
         <f t="shared" ca="1" si="0"/>
-        <v>20.664492616574361</v>
+        <v>20.723031107517805</v>
       </c>
     </row>
     <row r="53" spans="2:2" ht="15.75" customHeight="1">
       <c r="B53">
         <f t="shared" ca="1" si="0"/>
-        <v>19.129898968726998</v>
+        <v>20.68520748055197</v>
       </c>
     </row>
     <row r="54" spans="2:2" ht="15.75" customHeight="1">
       <c r="B54">
         <f t="shared" ca="1" si="0"/>
-        <v>18.690116028792804</v>
+        <v>22.068904024297414</v>
       </c>
     </row>
     <row r="55" spans="2:2" ht="15.75" customHeight="1">
       <c r="B55">
         <f t="shared" ca="1" si="0"/>
-        <v>16.677338981522688</v>
+        <v>24.011548346851328</v>
       </c>
     </row>
     <row r="56" spans="2:2" ht="15.75" customHeight="1">
       <c r="B56">
         <f t="shared" ca="1" si="0"/>
-        <v>17.138390850766015</v>
+        <v>21.966565210104037</v>
       </c>
     </row>
     <row r="57" spans="2:2" ht="15.75" customHeight="1">
       <c r="B57">
         <f t="shared" ca="1" si="0"/>
-        <v>17.557842812418617</v>
+        <v>21.396425223195621</v>
       </c>
     </row>
     <row r="58" spans="2:2" ht="15.75" customHeight="1">
       <c r="B58">
         <f t="shared" ca="1" si="0"/>
-        <v>17.457280314545315</v>
+        <v>20.00838906661874</v>
       </c>
     </row>
     <row r="59" spans="2:2" ht="15.75" customHeight="1">
       <c r="B59">
         <f t="shared" ca="1" si="0"/>
-        <v>17.58396063135708</v>
+        <v>20.586970064562344</v>
       </c>
     </row>
     <row r="60" spans="2:2" ht="15.75" customHeight="1">
       <c r="B60">
         <f t="shared" ca="1" si="0"/>
-        <v>18.85673089605644</v>
+        <v>21.096799394188476</v>
       </c>
     </row>
   </sheetData>

</xml_diff>